<commit_message>
Saving to Git as a possible final draft
</commit_message>
<xml_diff>
--- a/Phage_Data.xlsx
+++ b/Phage_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Draco\Desktop\QuantBio\eda-BeauAyers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D900BA8A-1006-4B84-A8A4-ED000022128A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0DF4EE-B217-450B-990F-532AE20EB908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1326,16 +1326,16 @@
     <t>cluster</t>
   </si>
   <si>
-    <t>genome (bp)</t>
-  </si>
-  <si>
-    <t>gc%</t>
-  </si>
-  <si>
     <t>host</t>
   </si>
   <si>
     <t>phage</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>bp</t>
   </si>
 </sst>
 </file>
@@ -1706,7 +1706,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1719,19 +1721,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>432</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>